<commit_message>
Add Tasklist. Add Sample Data Full. Sample Data instruction and tool
</commit_message>
<xml_diff>
--- a/document/Tasklist.xlsx
+++ b/document/Tasklist.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Description</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>Sample data tool</t>
+  </si>
+  <si>
+    <t>Real Effort</t>
   </si>
 </sst>
 </file>
@@ -413,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,9 +430,10 @@
     <col min="4" max="4" width="9.140625" style="2"/>
     <col min="5" max="5" width="15.7109375" customWidth="1"/>
     <col min="6" max="6" width="15.28515625" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -445,8 +449,11 @@
       <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -463,7 +470,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -480,7 +487,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -497,7 +504,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -514,7 +521,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Add design: Home page
</commit_message>
<xml_diff>
--- a/document/Tasklist.xlsx
+++ b/document/Tasklist.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Description</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>Research AJAX for Problem Detail Page View</t>
+  </si>
+  <si>
+    <t>CANCELLED</t>
   </si>
 </sst>
 </file>
@@ -469,7 +472,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,6 +655,9 @@
       <c r="E7" t="s">
         <v>9</v>
       </c>
+      <c r="G7" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="H7" s="4" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>

</xml_diff>